<commit_message>
Add weights to regression
</commit_message>
<xml_diff>
--- a/IndustryMap.xlsx
+++ b/IndustryMap.xlsx
@@ -314,6 +314,11 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
@@ -322,11 +327,6 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -644,8 +644,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:E35"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" topLeftCell="A22" workbookViewId="0">
-      <selection activeCell="A31" sqref="A31"/>
+    <sheetView showGridLines="0" tabSelected="1" workbookViewId="0">
+      <selection activeCell="H12" sqref="H12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -677,16 +677,16 @@
       <c r="A2" s="2" t="s">
         <v>12</v>
       </c>
-      <c r="B2" s="5" t="s">
+      <c r="B2" s="8" t="s">
         <v>13</v>
       </c>
-      <c r="C2" s="5" t="s">
+      <c r="C2" s="8" t="s">
         <v>14</v>
       </c>
-      <c r="D2" s="6" t="s">
+      <c r="D2" s="9" t="s">
         <v>9</v>
       </c>
-      <c r="E2" s="4" t="s">
+      <c r="E2" s="7" t="s">
         <v>35</v>
       </c>
     </row>
@@ -694,19 +694,19 @@
       <c r="A3" s="2" t="s">
         <v>41</v>
       </c>
-      <c r="B3" s="5"/>
-      <c r="C3" s="5"/>
-      <c r="D3" s="6"/>
-      <c r="E3" s="4"/>
+      <c r="B3" s="8"/>
+      <c r="C3" s="8"/>
+      <c r="D3" s="9"/>
+      <c r="E3" s="7"/>
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A4" s="2" t="s">
         <v>22</v>
       </c>
-      <c r="B4" s="5"/>
-      <c r="C4" s="5"/>
-      <c r="D4" s="6"/>
-      <c r="E4" s="4"/>
+      <c r="B4" s="8"/>
+      <c r="C4" s="8"/>
+      <c r="D4" s="9"/>
+      <c r="E4" s="7"/>
     </row>
     <row r="5" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A5" s="2" t="s">
@@ -715,87 +715,87 @@
       <c r="B5" s="3" t="s">
         <v>64</v>
       </c>
-      <c r="C5" s="5"/>
-      <c r="D5" s="6"/>
-      <c r="E5" s="4"/>
+      <c r="C5" s="8"/>
+      <c r="D5" s="9"/>
+      <c r="E5" s="7"/>
     </row>
     <row r="6" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A6" s="7" t="s">
+      <c r="A6" s="4" t="s">
         <v>36</v>
       </c>
-      <c r="B6" s="5" t="s">
+      <c r="B6" s="8" t="s">
         <v>16</v>
       </c>
-      <c r="C6" s="5" t="s">
+      <c r="C6" s="8" t="s">
         <v>11</v>
       </c>
-      <c r="D6" s="6"/>
-      <c r="E6" s="4"/>
+      <c r="D6" s="9"/>
+      <c r="E6" s="7"/>
     </row>
     <row r="7" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A7" s="7" t="s">
+      <c r="A7" s="4" t="s">
         <v>38</v>
       </c>
-      <c r="B7" s="5"/>
-      <c r="C7" s="5"/>
-      <c r="D7" s="6"/>
-      <c r="E7" s="4"/>
+      <c r="B7" s="8"/>
+      <c r="C7" s="8"/>
+      <c r="D7" s="9"/>
+      <c r="E7" s="7"/>
     </row>
     <row r="8" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A8" s="7" t="s">
+      <c r="A8" s="4" t="s">
         <v>15</v>
       </c>
-      <c r="B8" s="5"/>
-      <c r="C8" s="5"/>
-      <c r="D8" s="6"/>
-      <c r="E8" s="4"/>
+      <c r="B8" s="8"/>
+      <c r="C8" s="8"/>
+      <c r="D8" s="9"/>
+      <c r="E8" s="7"/>
     </row>
     <row r="9" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A9" s="8" t="s">
+      <c r="A9" s="5" t="s">
         <v>39</v>
       </c>
-      <c r="B9" s="5"/>
-      <c r="C9" s="5"/>
-      <c r="D9" s="6"/>
-      <c r="E9" s="4"/>
+      <c r="B9" s="8"/>
+      <c r="C9" s="8"/>
+      <c r="D9" s="9"/>
+      <c r="E9" s="7"/>
     </row>
     <row r="10" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A10" s="7" t="s">
+      <c r="A10" s="4" t="s">
         <v>27</v>
       </c>
-      <c r="B10" s="5"/>
-      <c r="C10" s="5"/>
-      <c r="D10" s="6"/>
-      <c r="E10" s="4"/>
+      <c r="B10" s="8"/>
+      <c r="C10" s="8"/>
+      <c r="D10" s="9"/>
+      <c r="E10" s="7"/>
     </row>
     <row r="11" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A11" s="2" t="s">
         <v>42</v>
       </c>
-      <c r="B11" s="5" t="s">
+      <c r="B11" s="8" t="s">
         <v>43</v>
       </c>
-      <c r="C11" s="5"/>
-      <c r="D11" s="6"/>
-      <c r="E11" s="4"/>
+      <c r="C11" s="8"/>
+      <c r="D11" s="9"/>
+      <c r="E11" s="7"/>
     </row>
     <row r="12" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A12" s="2" t="s">
         <v>44</v>
       </c>
-      <c r="B12" s="5"/>
-      <c r="C12" s="5"/>
-      <c r="D12" s="6"/>
-      <c r="E12" s="4"/>
+      <c r="B12" s="8"/>
+      <c r="C12" s="8"/>
+      <c r="D12" s="9"/>
+      <c r="E12" s="7"/>
     </row>
     <row r="13" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A13" s="2" t="s">
         <v>47</v>
       </c>
-      <c r="B13" s="5"/>
-      <c r="C13" s="5"/>
-      <c r="D13" s="6"/>
-      <c r="E13" s="4"/>
+      <c r="B13" s="8"/>
+      <c r="C13" s="8"/>
+      <c r="D13" s="9"/>
+      <c r="E13" s="7"/>
     </row>
     <row r="14" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A14" s="2" t="s">
@@ -804,87 +804,87 @@
       <c r="B14" s="3" t="s">
         <v>20</v>
       </c>
-      <c r="C14" s="5"/>
-      <c r="D14" s="6"/>
-      <c r="E14" s="4"/>
+      <c r="C14" s="8"/>
+      <c r="D14" s="9"/>
+      <c r="E14" s="7"/>
     </row>
     <row r="15" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A15" s="2" t="s">
         <v>45</v>
       </c>
-      <c r="B15" s="5" t="s">
+      <c r="B15" s="8" t="s">
         <v>46</v>
       </c>
-      <c r="C15" s="5"/>
-      <c r="D15" s="6"/>
-      <c r="E15" s="4"/>
+      <c r="C15" s="8"/>
+      <c r="D15" s="9"/>
+      <c r="E15" s="7"/>
     </row>
     <row r="16" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A16" s="2" t="s">
         <v>62</v>
       </c>
-      <c r="B16" s="5"/>
-      <c r="C16" s="5"/>
-      <c r="D16" s="6"/>
-      <c r="E16" s="4"/>
+      <c r="B16" s="8"/>
+      <c r="C16" s="8"/>
+      <c r="D16" s="9"/>
+      <c r="E16" s="7"/>
     </row>
     <row r="17" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A17" s="2" t="s">
         <v>37</v>
       </c>
-      <c r="B17" s="5" t="s">
+      <c r="B17" s="8" t="s">
         <v>10</v>
       </c>
-      <c r="C17" s="5"/>
-      <c r="D17" s="6"/>
-      <c r="E17" s="4"/>
+      <c r="C17" s="8"/>
+      <c r="D17" s="9"/>
+      <c r="E17" s="7"/>
     </row>
     <row r="18" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A18" s="2" t="s">
         <v>21</v>
       </c>
-      <c r="B18" s="5"/>
-      <c r="C18" s="5"/>
-      <c r="D18" s="6"/>
-      <c r="E18" s="4"/>
+      <c r="B18" s="8"/>
+      <c r="C18" s="8"/>
+      <c r="D18" s="9"/>
+      <c r="E18" s="7"/>
     </row>
     <row r="19" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A19" s="2" t="s">
         <v>8</v>
       </c>
-      <c r="B19" s="5"/>
-      <c r="C19" s="5"/>
-      <c r="D19" s="6"/>
-      <c r="E19" s="4"/>
+      <c r="B19" s="8"/>
+      <c r="C19" s="8"/>
+      <c r="D19" s="9"/>
+      <c r="E19" s="7"/>
     </row>
     <row r="20" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A20" s="2" t="s">
         <v>65</v>
       </c>
-      <c r="B20" s="5" t="s">
+      <c r="B20" s="8" t="s">
         <v>66</v>
       </c>
-      <c r="C20" s="5"/>
-      <c r="D20" s="6"/>
-      <c r="E20" s="4"/>
+      <c r="C20" s="8"/>
+      <c r="D20" s="9"/>
+      <c r="E20" s="7"/>
     </row>
     <row r="21" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A21" s="2" t="s">
         <v>67</v>
       </c>
-      <c r="B21" s="5"/>
-      <c r="C21" s="5"/>
-      <c r="D21" s="6"/>
-      <c r="E21" s="4"/>
+      <c r="B21" s="8"/>
+      <c r="C21" s="8"/>
+      <c r="D21" s="9"/>
+      <c r="E21" s="7"/>
     </row>
     <row r="22" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A22" s="2" t="s">
         <v>68</v>
       </c>
-      <c r="B22" s="5"/>
-      <c r="C22" s="5"/>
-      <c r="D22" s="6"/>
-      <c r="E22" s="4"/>
+      <c r="B22" s="8"/>
+      <c r="C22" s="8"/>
+      <c r="D22" s="9"/>
+      <c r="E22" s="7"/>
     </row>
     <row r="23" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A23" s="2" t="s">
@@ -893,9 +893,9 @@
       <c r="B23" s="3" t="s">
         <v>54</v>
       </c>
-      <c r="C23" s="5"/>
-      <c r="D23" s="6"/>
-      <c r="E23" s="4"/>
+      <c r="C23" s="8"/>
+      <c r="D23" s="9"/>
+      <c r="E23" s="7"/>
     </row>
     <row r="24" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A24" s="2" t="s">
@@ -904,9 +904,9 @@
       <c r="B24" s="3" t="s">
         <v>70</v>
       </c>
-      <c r="C24" s="5"/>
-      <c r="D24" s="6"/>
-      <c r="E24" s="4"/>
+      <c r="C24" s="8"/>
+      <c r="D24" s="9"/>
+      <c r="E24" s="7"/>
     </row>
     <row r="25" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A25" s="2" t="s">
@@ -915,9 +915,9 @@
       <c r="B25" s="3" t="s">
         <v>18</v>
       </c>
-      <c r="C25" s="5"/>
-      <c r="D25" s="6"/>
-      <c r="E25" s="4"/>
+      <c r="C25" s="8"/>
+      <c r="D25" s="9"/>
+      <c r="E25" s="7"/>
     </row>
     <row r="26" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A26" s="2" t="s">
@@ -929,10 +929,10 @@
       <c r="C26" s="3" t="s">
         <v>26</v>
       </c>
-      <c r="D26" s="5" t="s">
+      <c r="D26" s="8" t="s">
         <v>24</v>
       </c>
-      <c r="E26" s="4"/>
+      <c r="E26" s="7"/>
     </row>
     <row r="27" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A27" s="2" t="s">
@@ -941,11 +941,11 @@
       <c r="B27" s="3" t="s">
         <v>49</v>
       </c>
-      <c r="C27" s="5" t="s">
+      <c r="C27" s="8" t="s">
         <v>50</v>
       </c>
-      <c r="D27" s="5"/>
-      <c r="E27" s="4"/>
+      <c r="D27" s="8"/>
+      <c r="E27" s="7"/>
     </row>
     <row r="28" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A28" s="2" t="s">
@@ -954,9 +954,9 @@
       <c r="B28" s="3" t="s">
         <v>52</v>
       </c>
-      <c r="C28" s="5"/>
-      <c r="D28" s="5"/>
-      <c r="E28" s="4"/>
+      <c r="C28" s="8"/>
+      <c r="D28" s="8"/>
+      <c r="E28" s="7"/>
     </row>
     <row r="29" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A29" s="2" t="s">
@@ -965,9 +965,9 @@
       <c r="B29" s="3" t="s">
         <v>56</v>
       </c>
-      <c r="C29" s="5"/>
-      <c r="D29" s="5"/>
-      <c r="E29" s="4"/>
+      <c r="C29" s="8"/>
+      <c r="D29" s="8"/>
+      <c r="E29" s="7"/>
     </row>
     <row r="30" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A30" s="2" t="s">
@@ -976,22 +976,22 @@
       <c r="B30" s="3" t="s">
         <v>58</v>
       </c>
-      <c r="C30" s="5"/>
-      <c r="D30" s="5"/>
-      <c r="E30" s="4"/>
+      <c r="C30" s="8"/>
+      <c r="D30" s="8"/>
+      <c r="E30" s="7"/>
     </row>
     <row r="31" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A31" s="7" t="s">
+      <c r="A31" s="5" t="s">
         <v>28</v>
       </c>
-      <c r="B31" s="9" t="s">
+      <c r="B31" s="6" t="s">
         <v>29</v>
       </c>
       <c r="C31" s="3" t="s">
         <v>30</v>
       </c>
-      <c r="D31" s="5"/>
-      <c r="E31" s="4"/>
+      <c r="D31" s="8"/>
+      <c r="E31" s="7"/>
     </row>
     <row r="32" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A32" s="2" t="s">
@@ -1003,8 +1003,8 @@
       <c r="C32" s="3" t="s">
         <v>61</v>
       </c>
-      <c r="D32" s="5"/>
-      <c r="E32" s="4"/>
+      <c r="D32" s="8"/>
+      <c r="E32" s="7"/>
     </row>
     <row r="33" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A33" s="2" t="s">
@@ -1016,32 +1016,32 @@
       <c r="C33" s="3" t="s">
         <v>33</v>
       </c>
-      <c r="D33" s="5"/>
-      <c r="E33" s="4"/>
+      <c r="D33" s="8"/>
+      <c r="E33" s="7"/>
     </row>
     <row r="34" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A34" s="2" t="s">
         <v>40</v>
       </c>
-      <c r="B34" s="5" t="s">
+      <c r="B34" s="8" t="s">
         <v>6</v>
       </c>
-      <c r="C34" s="5" t="s">
+      <c r="C34" s="8" t="s">
         <v>7</v>
       </c>
-      <c r="D34" s="5" t="s">
+      <c r="D34" s="8" t="s">
         <v>5</v>
       </c>
-      <c r="E34" s="4"/>
+      <c r="E34" s="7"/>
     </row>
     <row r="35" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A35" s="2" t="s">
         <v>4</v>
       </c>
-      <c r="B35" s="5"/>
-      <c r="C35" s="5"/>
-      <c r="D35" s="5"/>
-      <c r="E35" s="4"/>
+      <c r="B35" s="8"/>
+      <c r="C35" s="8"/>
+      <c r="D35" s="8"/>
+      <c r="E35" s="7"/>
     </row>
   </sheetData>
   <sortState ref="A2:E35">

</xml_diff>